<commit_message>
creacion base de datos
</commit_message>
<xml_diff>
--- a/Documentación/Diagramas/Diccionario de Datos.xlsx
+++ b/Documentación/Diagramas/Diccionario de Datos.xlsx
@@ -222,9 +222,6 @@
     <t>PROPINA</t>
   </si>
   <si>
-    <t>TIME</t>
-  </si>
-  <si>
     <t>FK(EMPLEADO)</t>
   </si>
   <si>
@@ -298,6 +295,9 @@
   </si>
   <si>
     <t>FK(STOCK)</t>
+  </si>
+  <si>
+    <t>CHAR(5)</t>
   </si>
 </sst>
 </file>
@@ -835,7 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="A79" sqref="A79:C79"/>
     </sheetView>
   </sheetViews>
@@ -1419,7 +1419,7 @@
         <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C64" s="6"/>
     </row>
@@ -1428,7 +1428,7 @@
         <v>66</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C65" s="6"/>
     </row>
@@ -1449,19 +1449,19 @@
         <v>10</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1">
       <c r="A68" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68" s="11"/>
       <c r="C68" s="12"/>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>19</v>
@@ -1498,19 +1498,19 @@
         <v>10</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1">
       <c r="A73" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>19</v>
@@ -1530,14 +1530,14 @@
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1">
       <c r="A76" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="12"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>19</v>
@@ -1557,14 +1557,14 @@
     </row>
     <row r="79" spans="1:3" ht="15.75" thickBot="1">
       <c r="A79" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" s="11"/>
       <c r="C79" s="12"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>19</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>38</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>13</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>47</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>47</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>47</v>
@@ -1626,41 +1626,41 @@
         <v>10</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" thickBot="1">
       <c r="A88" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1">
       <c r="A89" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B89" s="11"/>
       <c r="C89" s="12"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>19</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>13</v>
@@ -1691,14 +1691,14 @@
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1">
       <c r="A93" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B93" s="11"/>
       <c r="C93" s="12"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>19</v>
@@ -1718,14 +1718,14 @@
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1">
       <c r="A96" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B96" s="11"/>
       <c r="C96" s="12"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>19</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>13</v>
@@ -1754,13 +1754,13 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1782,11 +1782,22 @@
         <v>10</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A49:C49"/>
     <mergeCell ref="A93:C93"/>
     <mergeCell ref="A96:C96"/>
     <mergeCell ref="A61:C61"/>
@@ -1795,17 +1806,6 @@
     <mergeCell ref="A76:C76"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A24:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modificacion base de datos
</commit_message>
<xml_diff>
--- a/Documentación/Diagramas/Diccionario de Datos.xlsx
+++ b/Documentación/Diagramas/Diccionario de Datos.xlsx
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:C79"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1524,7 +1524,7 @@
         <v>23</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C75" s="9"/>
     </row>
@@ -1712,7 +1712,7 @@
         <v>23</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C95" s="9"/>
     </row>

</xml_diff>